<commit_message>
Correct branched alkane parameters for Potoff.
</commit_message>
<xml_diff>
--- a/Results/data_tabulation.xlsx
+++ b/Results/data_tabulation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="42">
   <si>
     <t>Compound</t>
   </si>
@@ -92,9 +92,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>RUNNING</t>
-  </si>
-  <si>
     <t>NO (?)</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>NEVER (?)</t>
+  </si>
+  <si>
+    <t>C16H34</t>
   </si>
 </sst>
 </file>
@@ -541,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:O23"/>
+  <dimension ref="C1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20:H21"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +557,7 @@
     <col min="7" max="7" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -571,34 +571,37 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>
       </c>
       <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
       <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>3</v>
       </c>
@@ -617,9 +620,6 @@
       <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
       <c r="J2" t="s">
         <v>19</v>
       </c>
@@ -636,15 +636,18 @@
         <v>19</v>
       </c>
       <c r="O2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -656,10 +659,7 @@
         <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
@@ -667,11 +667,11 @@
       <c r="K3" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="N3" t="s">
         <v>19</v>
@@ -679,8 +679,11 @@
       <c r="O3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -699,70 +702,70 @@
       <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" t="s">
-        <v>38</v>
-      </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="M4" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="N4" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="O4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M5" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="N5" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="O5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="P5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -781,29 +784,30 @@
       <c r="H6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" t="s">
-        <v>19</v>
+      <c r="I6" s="5"/>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="L6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="O6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>7</v>
       </c>
@@ -822,29 +826,30 @@
       <c r="H7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" t="s">
-        <v>39</v>
+      <c r="I7" s="5"/>
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="L7" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="M7" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="N7" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="O7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>8</v>
       </c>
@@ -863,70 +868,71 @@
       <c r="H8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" t="s">
-        <v>19</v>
+      <c r="I8" s="5"/>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="L8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="O8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="M9" t="s">
+        <v>38</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="O9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="P9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>1</v>
       </c>
@@ -945,9 +951,6 @@
       <c r="H10" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="J10" s="5" t="s">
         <v>21</v>
       </c>
@@ -966,8 +969,11 @@
       <c r="O10" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>2</v>
       </c>
@@ -986,9 +992,6 @@
       <c r="H11" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="J11" s="5" t="s">
         <v>21</v>
       </c>
@@ -1007,91 +1010,94 @@
       <c r="O11" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" t="s">
-        <v>41</v>
-      </c>
       <c r="K12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="M12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="P12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparing to merge with updated script.
</commit_message>
<xml_diff>
--- a/Results/data_tabulation.xlsx
+++ b/Results/data_tabulation.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18570" windowHeight="9030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18570" windowHeight="9030" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Master list" sheetId="1" r:id="rId1"/>
+    <sheet name="State Point Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="119">
   <si>
     <t>Compound</t>
   </si>
@@ -92,9 +93,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>RUNNING</t>
-  </si>
-  <si>
     <t>NO (?)</t>
   </si>
   <si>
@@ -150,6 +148,240 @@
   </si>
   <si>
     <t>NEVER (?)</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Force Field</t>
+  </si>
+  <si>
+    <t>Point 1</t>
+  </si>
+  <si>
+    <t>Point 2</t>
+  </si>
+  <si>
+    <t>Point 3</t>
+  </si>
+  <si>
+    <t>Point 4</t>
+  </si>
+  <si>
+    <t>Point 5</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Potential issues</t>
+  </si>
+  <si>
+    <t>Saturation</t>
+  </si>
+  <si>
+    <t>TAMie</t>
+  </si>
+  <si>
+    <t>md1 (ram9)</t>
+  </si>
+  <si>
+    <t>Likely run with old bootstrap script</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>TraPPE</t>
+  </si>
+  <si>
+    <t>Starts at point 5, goes to 9</t>
+  </si>
+  <si>
+    <t>OK (odd plateau)</t>
+  </si>
+  <si>
+    <t>Potoff</t>
+  </si>
+  <si>
+    <t>Point 6</t>
+  </si>
+  <si>
+    <t>Point 7</t>
+  </si>
+  <si>
+    <t>Point 8</t>
+  </si>
+  <si>
+    <t>skewed</t>
+  </si>
+  <si>
+    <t>Likely run with old bootstrap script (40 replicates only)</t>
+  </si>
+  <si>
+    <t>T293highP</t>
+  </si>
+  <si>
+    <t>30 Replicates only, 800 molecules</t>
+  </si>
+  <si>
+    <t>Useless plots</t>
+  </si>
+  <si>
+    <t>30 Replictates only, 200 molecules</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Point 0</t>
+  </si>
+  <si>
+    <t>Uselss plots</t>
+  </si>
+  <si>
+    <t>Bad fit</t>
+  </si>
+  <si>
+    <t>Useless plot</t>
+  </si>
+  <si>
+    <t>Bizare</t>
+  </si>
+  <si>
+    <t>Collaborator</t>
+  </si>
+  <si>
+    <t>bimodal</t>
+  </si>
+  <si>
+    <t>bimodal/poor fit</t>
+  </si>
+  <si>
+    <t>OK (noisy)</t>
+  </si>
+  <si>
+    <t>Likely run with old boostrap script</t>
+  </si>
+  <si>
+    <t>Sim. Too short</t>
+  </si>
+  <si>
+    <t>Only 40 reps; run with old boostrap likely</t>
+  </si>
+  <si>
+    <t>Collaborator (?)</t>
+  </si>
+  <si>
+    <t>Bimodal</t>
+  </si>
+  <si>
+    <t>Plot error</t>
+  </si>
+  <si>
+    <t>40 replicates; likely run with old bootstrap</t>
+  </si>
+  <si>
+    <t>OK (poor fit)</t>
+  </si>
+  <si>
+    <t>bad fit</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>bad fit/bimodal</t>
+  </si>
+  <si>
+    <t>run too short</t>
+  </si>
+  <si>
+    <t>run too short/failed run</t>
+  </si>
+  <si>
+    <t>poor fit</t>
+  </si>
+  <si>
+    <t>md1 (mca1)</t>
+  </si>
+  <si>
+    <t>OK (bimodal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK  </t>
+  </si>
+  <si>
+    <t>AUA4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK </t>
+  </si>
+  <si>
+    <t>OK (funny bootstrap)</t>
+  </si>
+  <si>
+    <t>Poor fit</t>
+  </si>
+  <si>
+    <t>Refused to run</t>
+  </si>
+  <si>
+    <t>Useless fit</t>
+  </si>
+  <si>
+    <t>Bad fit/bimodal</t>
+  </si>
+  <si>
+    <t>Poor fit/bimodal</t>
+  </si>
+  <si>
+    <t>May have used old bootstrap script/bad top file</t>
+  </si>
+  <si>
+    <t>Run too short</t>
+  </si>
+  <si>
+    <t>Skewed</t>
+  </si>
+  <si>
+    <t>Useless plot/poor fit</t>
+  </si>
+  <si>
+    <t>23DMButane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saturation </t>
+  </si>
+  <si>
+    <t>OK (useless plot)</t>
+  </si>
+  <si>
+    <t>3MPentane</t>
+  </si>
+  <si>
+    <t>Funny bootstrap</t>
+  </si>
+  <si>
+    <t>Poor fit/Funny bootstraps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">md1 (ram9) </t>
+  </si>
+  <si>
+    <t>OK (weird)</t>
+  </si>
+  <si>
+    <t>awful fit</t>
+  </si>
+  <si>
+    <t>Reran</t>
+  </si>
+  <si>
+    <t>To rerun</t>
+  </si>
+  <si>
+    <t>Reran-still broken</t>
   </si>
 </sst>
 </file>
@@ -200,12 +432,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -220,13 +470,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20:H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +825,7 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>
@@ -586,7 +840,7 @@
         <v>18</v>
       </c>
       <c r="L1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M1" t="s">
         <v>14</v>
@@ -636,7 +890,7 @@
         <v>19</v>
       </c>
       <c r="O2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="3:15" x14ac:dyDescent="0.25">
@@ -644,7 +898,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -656,7 +910,7 @@
         <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
@@ -700,19 +954,19 @@
         <v>19</v>
       </c>
       <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
         <v>38</v>
       </c>
-      <c r="J4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" t="s">
-        <v>39</v>
-      </c>
       <c r="L4" t="s">
         <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N4" t="s">
         <v>19</v>
@@ -723,43 +977,43 @@
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
         <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M5" t="s">
         <v>19</v>
       </c>
       <c r="N5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.25">
@@ -785,7 +1039,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K6" t="s">
         <v>19</v>
@@ -826,16 +1080,16 @@
         <v>19</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L7" t="s">
         <v>21</v>
       </c>
       <c r="M7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N7" t="s">
         <v>21</v>
@@ -867,7 +1121,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K8" t="s">
         <v>19</v>
@@ -887,43 +1141,43 @@
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" t="s">
         <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="N9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="3:15" x14ac:dyDescent="0.25">
@@ -1010,88 +1264,1721 @@
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" t="s">
-        <v>41</v>
-      </c>
       <c r="J12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" t="s">
+        <v>54</v>
+      </c>
+      <c r="L10" t="s">
+        <v>71</v>
+      </c>
+      <c r="M10" t="s">
+        <v>72</v>
+      </c>
+      <c r="N10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" t="s">
+        <v>72</v>
+      </c>
+      <c r="M12" t="s">
+        <v>54</v>
+      </c>
+      <c r="N12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17" t="s">
+        <v>54</v>
+      </c>
+      <c r="L17" t="s">
+        <v>54</v>
+      </c>
+      <c r="M17" t="s">
+        <v>79</v>
+      </c>
+      <c r="N17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I19" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" t="s">
+        <v>85</v>
+      </c>
+      <c r="J21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" t="s">
+        <v>88</v>
+      </c>
+      <c r="I22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" t="s">
+        <v>93</v>
+      </c>
+      <c r="I26" t="s">
+        <v>54</v>
+      </c>
+      <c r="J26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" t="s">
+        <v>54</v>
+      </c>
+      <c r="J27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" t="s">
+        <v>54</v>
+      </c>
+      <c r="J28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" t="s">
+        <v>98</v>
+      </c>
+      <c r="J29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" t="s">
+        <v>54</v>
+      </c>
+      <c r="J30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H31" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" t="s">
+        <v>54</v>
+      </c>
+      <c r="J31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" t="s">
+        <v>54</v>
+      </c>
+      <c r="J32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" t="s">
+        <v>72</v>
+      </c>
+      <c r="H33" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" t="s">
+        <v>54</v>
+      </c>
+      <c r="J33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" t="s">
+        <v>113</v>
+      </c>
+      <c r="F35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H35" t="s">
+        <v>54</v>
+      </c>
+      <c r="I35" t="s">
+        <v>54</v>
+      </c>
+      <c r="J35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" t="s">
+        <v>101</v>
+      </c>
+      <c r="G37" t="s">
+        <v>54</v>
+      </c>
+      <c r="H37" t="s">
+        <v>54</v>
+      </c>
+      <c r="I37" t="s">
+        <v>85</v>
+      </c>
+      <c r="J37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38" t="s">
+        <v>54</v>
+      </c>
+      <c r="J38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E40" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H40" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" t="s">
+        <v>54</v>
+      </c>
+      <c r="J40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" t="s">
+        <v>54</v>
+      </c>
+      <c r="G41" t="s">
+        <v>54</v>
+      </c>
+      <c r="H41" t="s">
+        <v>54</v>
+      </c>
+      <c r="I41" t="s">
+        <v>85</v>
+      </c>
+      <c r="J41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" t="s">
+        <v>54</v>
+      </c>
+      <c r="G42" t="s">
+        <v>54</v>
+      </c>
+      <c r="H42" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42" t="s">
+        <v>98</v>
+      </c>
+      <c r="J42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>33</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" t="s">
+        <v>96</v>
+      </c>
+      <c r="G45" t="s">
+        <v>54</v>
+      </c>
+      <c r="H45" t="s">
+        <v>54</v>
+      </c>
+      <c r="I45" t="s">
+        <v>54</v>
+      </c>
+      <c r="J45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" t="s">
+        <v>106</v>
+      </c>
+      <c r="G46" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" t="s">
+        <v>54</v>
+      </c>
+      <c r="I46" t="s">
+        <v>54</v>
+      </c>
+      <c r="J46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" t="s">
+        <v>54</v>
+      </c>
+      <c r="G47" t="s">
+        <v>54</v>
+      </c>
+      <c r="H47" t="s">
+        <v>54</v>
+      </c>
+      <c r="I47" t="s">
+        <v>54</v>
+      </c>
+      <c r="J47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F48" t="s">
+        <v>54</v>
+      </c>
+      <c r="G48" t="s">
+        <v>54</v>
+      </c>
+      <c r="H48" t="s">
+        <v>54</v>
+      </c>
+      <c r="I48" t="s">
+        <v>54</v>
+      </c>
+      <c r="J48" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50" t="s">
+        <v>54</v>
+      </c>
+      <c r="H50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I50" t="s">
+        <v>54</v>
+      </c>
+      <c r="J50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" t="s">
+        <v>54</v>
+      </c>
+      <c r="G51" t="s">
+        <v>54</v>
+      </c>
+      <c r="H51" t="s">
+        <v>111</v>
+      </c>
+      <c r="I51" t="s">
+        <v>54</v>
+      </c>
+      <c r="J51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D53" t="s">
+        <v>92</v>
+      </c>
+      <c r="F53" t="s">
+        <v>112</v>
+      </c>
+      <c r="G53" t="s">
+        <v>54</v>
+      </c>
+      <c r="H53" t="s">
+        <v>54</v>
+      </c>
+      <c r="I53" t="s">
+        <v>77</v>
+      </c>
+      <c r="J53" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>